<commit_message>
duplikaattien ja parin muun virhearvon korjaus
</commit_message>
<xml_diff>
--- a/style_ids.xlsx
+++ b/style_ids.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\mtb-trailmap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49BB8D27-2110-40EE-BC89-0712C02DF0E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C4E4DE-A31A-484A-BB76-F7CBF1B0A3F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{C589A0E4-6D1B-4D89-868D-0F4B65CA5C94}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3235" uniqueCount="677">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3236" uniqueCount="677">
   <si>
     <t>background</t>
   </si>
@@ -2941,7 +2941,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E326" sqref="E326:E327"/>
+      <selection pane="bottomLeft" activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -3557,13 +3557,16 @@
       </c>
       <c r="B25" t="str">
         <f t="shared" si="0"/>
-        <v>landcover-scrub-(def-all-osm)</v>
+        <v>landcover-scrub-nowoods-(def-all-osm)</v>
       </c>
       <c r="C25" t="s">
         <v>416</v>
       </c>
       <c r="D25" t="s">
         <v>417</v>
+      </c>
+      <c r="E25" t="s">
+        <v>426</v>
       </c>
       <c r="F25" t="s">
         <v>448</v>
@@ -8510,7 +8513,7 @@
       </c>
       <c r="B198" t="str">
         <f t="shared" si="3"/>
-        <v>highway-trunk-case-(def-all-osm)</v>
+        <v>highway-trunk-case-(wnt-all-osm)</v>
       </c>
       <c r="C198" t="s">
         <v>550</v>
@@ -8522,7 +8525,7 @@
         <v>451</v>
       </c>
       <c r="F198" t="s">
-        <v>448</v>
+        <v>553</v>
       </c>
       <c r="G198" t="s">
         <v>658</v>
@@ -8540,7 +8543,7 @@
       </c>
       <c r="B199" t="str">
         <f t="shared" si="3"/>
-        <v>highway-trunk-case-(wnt-all-osm)</v>
+        <v>highway-trunk-case-(gr-all-osm)</v>
       </c>
       <c r="C199" t="s">
         <v>550</v>
@@ -8552,7 +8555,7 @@
         <v>451</v>
       </c>
       <c r="F199" t="s">
-        <v>553</v>
+        <v>421</v>
       </c>
       <c r="G199" t="s">
         <v>658</v>
@@ -10019,7 +10022,7 @@
       </c>
       <c r="B247" t="str">
         <f t="shared" si="3"/>
-        <v>access-bicycle_winter-no-(def-all-osm)</v>
+        <v>access-bicycle_winter-no-(wnt-all-osm)</v>
       </c>
       <c r="C247" t="s">
         <v>552</v>
@@ -10031,7 +10034,7 @@
         <v>563</v>
       </c>
       <c r="F247" t="s">
-        <v>448</v>
+        <v>553</v>
       </c>
       <c r="G247" t="s">
         <v>658</v>

</xml_diff>